<commit_message>
Change c to x in ion documents
</commit_message>
<xml_diff>
--- a/Data_ions/Perovskite_ions_data.xlsx
+++ b/Data_ions/Perovskite_ions_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesja78\Dropbox\Dokument Jobbet Linköping\PROJECT\Jacobsson - 2023 - Perovskite A cations\Code_v5\Data_ions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1391171-AF6C-428B-A5B2-BA5D9CD912C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC483218-8EF9-4C2F-B9CF-951B7A8DEB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{115B1035-8E8F-436F-AAFE-3FEDDF124ACA}"/>
   </bookViews>
@@ -8041,9 +8041,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>abbreviation</t>
   </si>
   <si>
@@ -8180,6 +8177,9 @@
   </si>
   <si>
     <t>Au+3</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -8848,7 +8848,7 @@
   <dimension ref="A1:N336"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
-      <selection activeCell="F342" sqref="F342"/>
+      <selection activeCell="C341" sqref="C341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8874,43 +8874,43 @@
         <v>2272</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="C1" t="s">
+        <v>2555</v>
+      </c>
+      <c r="D1" t="s">
         <v>2556</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2557</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2558</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2559</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2560</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2561</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>2563</v>
+      </c>
+      <c r="K1" t="s">
         <v>2562</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="26" t="s">
         <v>2564</v>
       </c>
-      <c r="K1" t="s">
-        <v>2563</v>
-      </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="2" t="s">
+        <v>2566</v>
+      </c>
+      <c r="N1" t="s">
         <v>2565</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>2567</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2566</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8986,7 +8986,7 @@
         <v>17</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="M3" s="3">
         <v>36</v>
@@ -11513,7 +11513,7 @@
         <v>534</v>
       </c>
       <c r="L66" s="32" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="M66" s="3">
         <v>9</v>
@@ -20058,7 +20058,7 @@
         <v>2273</v>
       </c>
       <c r="E297" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="F297" t="s">
         <v>2274</v>
@@ -20096,7 +20096,7 @@
         <v>2280</v>
       </c>
       <c r="E298" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="F298" t="s">
         <v>2281</v>
@@ -20134,7 +20134,7 @@
         <v>2287</v>
       </c>
       <c r="E299" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="F299" t="s">
         <v>2288</v>
@@ -20172,7 +20172,7 @@
         <v>2294</v>
       </c>
       <c r="E300" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="F300" t="s">
         <v>2295</v>
@@ -20248,7 +20248,7 @@
         <v>2309</v>
       </c>
       <c r="E302" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="F302" t="s">
         <v>2310</v>
@@ -20286,7 +20286,7 @@
         <v>2316</v>
       </c>
       <c r="E303" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="F303" t="s">
         <v>2317</v>
@@ -20321,7 +20321,7 @@
         <v>2322</v>
       </c>
       <c r="E304" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="F304" t="s">
         <v>2323</v>
@@ -20359,7 +20359,7 @@
         <v>2329</v>
       </c>
       <c r="E305" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="F305" t="s">
         <v>2330</v>
@@ -20397,7 +20397,7 @@
         <v>2336</v>
       </c>
       <c r="E306" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="F306" t="s">
         <v>2337</v>
@@ -20435,7 +20435,7 @@
         <v>2343</v>
       </c>
       <c r="E307" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="F307" t="s">
         <v>2344</v>
@@ -20473,7 +20473,7 @@
         <v>2350</v>
       </c>
       <c r="E308" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="F308" t="s">
         <v>2351</v>
@@ -20511,7 +20511,7 @@
         <v>2357</v>
       </c>
       <c r="E309" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="F309" t="s">
         <v>2358</v>
@@ -20549,7 +20549,7 @@
         <v>2364</v>
       </c>
       <c r="E310" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="F310" t="s">
         <v>2365</v>
@@ -20587,7 +20587,7 @@
         <v>2371</v>
       </c>
       <c r="E311" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
       <c r="F311" t="s">
         <v>2372</v>
@@ -20625,7 +20625,7 @@
         <v>2378</v>
       </c>
       <c r="E312" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="F312" t="s">
         <v>2379</v>
@@ -20663,7 +20663,7 @@
         <v>2385</v>
       </c>
       <c r="E313" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="F313" t="s">
         <v>2386</v>
@@ -20701,7 +20701,7 @@
         <v>2392</v>
       </c>
       <c r="E314" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="F314" t="s">
         <v>2393</v>
@@ -20739,7 +20739,7 @@
         <v>2399</v>
       </c>
       <c r="E315" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="F315" t="s">
         <v>2400</v>
@@ -20777,7 +20777,7 @@
         <v>2406</v>
       </c>
       <c r="E316" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="F316" t="s">
         <v>2407</v>
@@ -20815,7 +20815,7 @@
         <v>18</v>
       </c>
       <c r="E317" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="F317" t="s">
         <v>2413</v>
@@ -20853,7 +20853,7 @@
         <v>2416</v>
       </c>
       <c r="E318" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="F318" t="s">
         <v>2417</v>
@@ -20891,7 +20891,7 @@
         <v>2423</v>
       </c>
       <c r="E319" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
       <c r="F319" t="s">
         <v>2424</v>
@@ -20929,7 +20929,7 @@
         <v>2430</v>
       </c>
       <c r="E320" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="F320" t="s">
         <v>2431</v>
@@ -20967,7 +20967,7 @@
         <v>2436</v>
       </c>
       <c r="E321" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="F321" t="s">
         <v>2437</v>
@@ -21005,7 +21005,7 @@
         <v>2443</v>
       </c>
       <c r="E322" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="F322" t="s">
         <v>2444</v>
@@ -21043,7 +21043,7 @@
         <v>2449</v>
       </c>
       <c r="E323" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="F323" t="s">
         <v>2450</v>
@@ -21081,7 +21081,7 @@
         <v>2456</v>
       </c>
       <c r="E324" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="F324" t="s">
         <v>2457</v>
@@ -21119,7 +21119,7 @@
         <v>2463</v>
       </c>
       <c r="E325" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="F325" t="s">
         <v>2464</v>
@@ -21195,7 +21195,7 @@
         <v>2470</v>
       </c>
       <c r="E327" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="F327" t="s">
         <v>2478</v>
@@ -21227,7 +21227,7 @@
         <v>1</v>
       </c>
       <c r="B328" s="27" t="s">
-        <v>2555</v>
+        <v>2601</v>
       </c>
       <c r="C328" t="s">
         <v>2481</v>
@@ -21265,7 +21265,7 @@
         <v>2</v>
       </c>
       <c r="B329" s="27" t="s">
-        <v>2555</v>
+        <v>2601</v>
       </c>
       <c r="C329" t="s">
         <v>2489</v>
@@ -21303,7 +21303,7 @@
         <v>3</v>
       </c>
       <c r="B330" s="27" t="s">
-        <v>2555</v>
+        <v>2601</v>
       </c>
       <c r="C330" t="s">
         <v>2497</v>
@@ -21341,13 +21341,13 @@
         <v>4</v>
       </c>
       <c r="B331" s="27" t="s">
-        <v>2555</v>
+        <v>2601</v>
       </c>
       <c r="C331" t="s">
         <v>2505</v>
       </c>
       <c r="E331" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="F331" t="s">
         <v>2506</v>
@@ -21379,13 +21379,13 @@
         <v>5</v>
       </c>
       <c r="B332" s="27" t="s">
-        <v>2555</v>
+        <v>2601</v>
       </c>
       <c r="C332" t="s">
         <v>2513</v>
       </c>
       <c r="E332" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="F332" t="s">
         <v>2514</v>
@@ -21417,7 +21417,7 @@
         <v>6</v>
       </c>
       <c r="B333" s="27" t="s">
-        <v>2555</v>
+        <v>2601</v>
       </c>
       <c r="C333" t="s">
         <v>2520</v>
@@ -21455,7 +21455,7 @@
         <v>7</v>
       </c>
       <c r="B334" s="27" t="s">
-        <v>2555</v>
+        <v>2601</v>
       </c>
       <c r="C334" t="s">
         <v>2528</v>
@@ -21493,7 +21493,7 @@
         <v>8</v>
       </c>
       <c r="B335" s="27" t="s">
-        <v>2555</v>
+        <v>2601</v>
       </c>
       <c r="C335" t="s">
         <v>2537</v>
@@ -21531,7 +21531,7 @@
         <v>9</v>
       </c>
       <c r="B336" s="27" t="s">
-        <v>2555</v>
+        <v>2601</v>
       </c>
       <c r="C336" t="s">
         <v>2545</v>

</xml_diff>